<commit_message>
con la ultima tarea...
</commit_message>
<xml_diff>
--- a/CAPITULO 2/Ejemplo recomendaciones.xlsx
+++ b/CAPITULO 2/Ejemplo recomendaciones.xlsx
@@ -570,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,179 +888,184 @@
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="9">
-        <v>0.41</v>
-      </c>
-      <c r="C22" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="D22" s="13">
-        <f>B22*C22</f>
-        <v>1.845</v>
-      </c>
-      <c r="E22" s="12">
-        <v>3</v>
-      </c>
-      <c r="F22" s="13">
-        <f>B22*E22</f>
-        <v>1.23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="9">
-        <v>0.37</v>
+        <v>0.41</v>
       </c>
       <c r="C23" s="12">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D23" s="13">
-        <f t="shared" ref="D23:D26" si="2">B23*C23</f>
-        <v>1.85</v>
-      </c>
-      <c r="E23" s="12"/>
+        <f>B23*C23</f>
+        <v>1.845</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
       <c r="F23" s="13">
-        <f t="shared" ref="F23:F26" si="3">B23*E23</f>
-        <v>0</v>
+        <f>B23*E23</f>
+        <v>1.23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="9">
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="C24" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="13">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="E24" s="12">
-        <v>3</v>
-      </c>
+        <f t="shared" ref="D24:D27" si="2">B24*C24</f>
+        <v>1.85</v>
+      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="13">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" ref="F24:F27" si="3">B24*E24</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" s="9">
-        <v>0.31</v>
+        <v>1</v>
       </c>
       <c r="C25" s="12">
         <v>4</v>
       </c>
       <c r="D25" s="13">
         <f t="shared" si="2"/>
-        <v>1.24</v>
+        <v>4</v>
       </c>
       <c r="E25" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="13">
         <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.31</v>
+      </c>
+      <c r="C26" s="12">
+        <v>4</v>
+      </c>
+      <c r="D26" s="13">
+        <f t="shared" si="2"/>
+        <v>1.24</v>
+      </c>
+      <c r="E26" s="12">
+        <v>2</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="3"/>
         <v>0.62</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="9">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="9">
         <v>0.5</v>
       </c>
-      <c r="C26" s="14">
-        <v>4</v>
-      </c>
-      <c r="D26" s="15">
+      <c r="C27" s="14">
+        <v>4</v>
+      </c>
+      <c r="D27" s="15">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E26" s="14">
-        <v>4</v>
-      </c>
-      <c r="F26" s="15">
+      <c r="E27" s="14">
+        <v>4</v>
+      </c>
+      <c r="F27" s="15">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="D27" s="3">
-        <f>SUM(D22:D26)</f>
-        <v>10.935</v>
-      </c>
-      <c r="F27" s="3">
-        <f>SUM(F22:F26)</f>
-        <v>6.8500000000000005</v>
-      </c>
-    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B28" s="3"/>
       <c r="D28" s="3">
-        <f>SUM(B22:B26)</f>
-        <v>2.59</v>
+        <f>SUM(D23:D27)</f>
+        <v>10.935</v>
       </c>
       <c r="F28" s="3">
-        <f>SUM(B22,B24:B26)</f>
-        <v>2.2199999999999998</v>
+        <f>SUM(F23:F27)</f>
+        <v>6.8500000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3">
+        <f>SUM(B23:B27)</f>
+        <v>2.59</v>
+      </c>
+      <c r="F29" s="3">
+        <f>SUM(B23,B25:B27)</f>
+        <v>2.2199999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="7">
-        <f>D27/D28</f>
+      <c r="D30" s="7">
+        <f>D28/D29</f>
         <v>4.2220077220077226</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7">
-        <f>F27/F28</f>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7">
+        <f>F28/F29</f>
         <v>3.0855855855855863</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregadas las recomendaciones por items en el ejemplo de excel
</commit_message>
<xml_diff>
--- a/CAPITULO 2/Ejemplo recomendaciones.xlsx
+++ b/CAPITULO 2/Ejemplo recomendaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9795" windowHeight="5310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
   <si>
     <t>jesica</t>
   </si>
@@ -60,21 +60,6 @@
     <t>wz</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>jose</t>
-  </si>
-  <si>
-    <t>carlos</t>
-  </si>
-  <si>
-    <t>juan</t>
-  </si>
-  <si>
     <t>pearson</t>
   </si>
   <si>
@@ -103,6 +88,27 @@
   </si>
   <si>
     <t>PARA MABEL(distancia de pearson)</t>
+  </si>
+  <si>
+    <t>PREDICCIONES PARA MABEL</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>R x rapfur</t>
+  </si>
+  <si>
+    <t>R x wz</t>
+  </si>
+  <si>
+    <t>RECOMENDACIONES BASADAS EN USUARIOS</t>
+  </si>
+  <si>
+    <t>RECOMENDACIONES BASADAS EN ITEMS</t>
+  </si>
+  <si>
+    <t>tabla de similitudes</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +135,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -272,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -290,6 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,490 +598,500 @@
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C4" s="4">
         <v>4.5</v>
       </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>4</v>
-      </c>
       <c r="D4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>4</v>
-      </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4</v>
+      </c>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B13" s="8">
         <v>-1</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C13" s="4">
         <v>4.5</v>
       </c>
-      <c r="D11" s="5">
-        <f>B11*C11</f>
+      <c r="D13" s="5">
+        <f>B13*C13</f>
         <v>-4.5</v>
       </c>
-      <c r="E11" s="4">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5">
-        <f>B11*E11</f>
+      <c r="E13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <f>B13*E13</f>
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="5">
-        <f>PEARSON(C3:G3,C7:G7)</f>
+      <c r="B14" s="5">
+        <f>PEARSON(C5:G5,C9:G9)</f>
         <v>0.6546536707079772</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="5">
-        <f t="shared" ref="D12:D15" si="0">B12*C12</f>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14:D17" si="0">B14*C14</f>
         <v>3.2732683535398861</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5">
-        <f t="shared" ref="F12:F15" si="1">B12*E12</f>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5">
+        <f t="shared" ref="F14:F17" si="1">B14*E14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5">
-        <f>PEARSON(C7:G7,C4:G4)</f>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5">
+        <f>PEARSON(C9:G9,C6:G6)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="4">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E13" s="4">
-        <v>3</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5">
-        <f>PEARSON(C7:G7,C5:G5)</f>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5">
+        <f>PEARSON(C9:G9,C7:G7)</f>
         <v>0.3273268353539886</v>
       </c>
-      <c r="C14" s="4">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>1.3093073414159544</v>
       </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>0.6546536707079772</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5">
-        <f>PEARSON(C7:G7,C6:G6)</f>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <f>PEARSON(C9:G9,C8:G8)</f>
         <v>0.8660254037844386</v>
       </c>
-      <c r="C15" s="4">
-        <v>4</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>3.4641016151377544</v>
       </c>
-      <c r="E15" s="4">
-        <v>4</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="E17" s="4">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
         <f t="shared" si="1"/>
         <v>3.4641016151377544</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3">
-        <f>SUM(D11:D15)</f>
-        <v>7.5466773100935951</v>
-      </c>
-      <c r="F16" s="3">
-        <f>SUM(F11:F15)</f>
-        <v>4.1187552858457313</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3">
-        <f>SUM(B11:B15)</f>
-        <v>1.8480059098464043</v>
-      </c>
-      <c r="F17" s="3">
-        <f>SUM(B11,B13:B15)</f>
-        <v>1.1933522391384273</v>
-      </c>
-    </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="7">
-        <f>D16/D17</f>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <f>SUM(D13:D17)</f>
+        <v>7.5466773100935951</v>
+      </c>
+      <c r="F18" s="3">
+        <f>SUM(F13:F17)</f>
+        <v>4.1187552858457313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <f>SUM(B13:B17)</f>
+        <v>1.8480059098464043</v>
+      </c>
+      <c r="F19" s="3">
+        <f>SUM(B13,B15:B17)</f>
+        <v>1.1933522391384273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="7">
+        <f>D18/D19</f>
         <v>4.0836867836211797</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7">
-        <f>F16/F17</f>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7">
+        <f>F18/F19</f>
         <v>3.4514162296451358</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="D24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="9">
-        <v>0.41</v>
-      </c>
-      <c r="C23" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="D23" s="13">
-        <f>B23*C23</f>
-        <v>1.845</v>
-      </c>
-      <c r="E23" s="12">
-        <v>3</v>
-      </c>
-      <c r="F23" s="13">
-        <f>B23*E23</f>
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0.37</v>
-      </c>
-      <c r="C24" s="12">
-        <v>5</v>
-      </c>
-      <c r="D24" s="13">
-        <f t="shared" ref="D24:D27" si="2">B24*C24</f>
-        <v>1.85</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13">
-        <f t="shared" ref="F24:F27" si="3">B24*E24</f>
-        <v>0</v>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B25" s="9">
-        <v>1</v>
+        <v>0.41</v>
       </c>
       <c r="C25" s="12">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D25" s="13">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>B25*C25</f>
+        <v>1.845</v>
       </c>
       <c r="E25" s="12">
         <v>3</v>
       </c>
       <c r="F25" s="13">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f>B25*E25</f>
+        <v>1.23</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" s="9">
+        <v>0.37</v>
+      </c>
+      <c r="C26" s="12">
+        <v>5</v>
+      </c>
+      <c r="D26" s="13">
+        <f t="shared" ref="D26:D29" si="2">B26*C26</f>
+        <v>1.85</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13">
+        <f t="shared" ref="F26:F29" si="3">B26*E26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12">
+        <v>4</v>
+      </c>
+      <c r="D27" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E27" s="12">
+        <v>3</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="9">
         <v>0.31</v>
       </c>
-      <c r="C26" s="12">
-        <v>4</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="C28" s="12">
+        <v>4</v>
+      </c>
+      <c r="D28" s="13">
         <f t="shared" si="2"/>
         <v>1.24</v>
       </c>
-      <c r="E26" s="12">
-        <v>2</v>
-      </c>
-      <c r="F26" s="13">
+      <c r="E28" s="12">
+        <v>2</v>
+      </c>
+      <c r="F28" s="13">
         <f t="shared" si="3"/>
         <v>0.62</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="9">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="9">
         <v>0.5</v>
       </c>
-      <c r="C27" s="14">
-        <v>4</v>
-      </c>
-      <c r="D27" s="15">
+      <c r="C29" s="14">
+        <v>4</v>
+      </c>
+      <c r="D29" s="15">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E27" s="14">
-        <v>4</v>
-      </c>
-      <c r="F27" s="15">
+      <c r="E29" s="14">
+        <v>4</v>
+      </c>
+      <c r="F29" s="15">
         <f t="shared" si="3"/>
         <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="D28" s="3">
-        <f>SUM(D23:D27)</f>
-        <v>10.935</v>
-      </c>
-      <c r="F28" s="3">
-        <f>SUM(F23:F27)</f>
-        <v>6.8500000000000005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="3">
-        <f>SUM(B23:B27)</f>
-        <v>2.59</v>
-      </c>
-      <c r="F29" s="3">
-        <f>SUM(B23,B25:B27)</f>
-        <v>2.2199999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="7">
-        <f>D28/D29</f>
+        <v>14</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="D30" s="3">
+        <f>SUM(D25:D29)</f>
+        <v>10.935</v>
+      </c>
+      <c r="F30" s="3">
+        <f>SUM(F25:F29)</f>
+        <v>6.8500000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3">
+        <f>SUM(B25:B29)</f>
+        <v>2.59</v>
+      </c>
+      <c r="F31" s="3">
+        <f>SUM(B25,B27:B29)</f>
+        <v>2.2199999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="7">
+        <f>D30/D31</f>
         <v>4.2220077220077226</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7">
-        <f>F28/F29</f>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7">
+        <f>F30/F31</f>
         <v>3.0855855855855863</v>
       </c>
     </row>
@@ -1077,78 +1103,382 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K12"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <f>LOOKUP(I4,B4:B6,C4:C6)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H9">
-        <v>12</v>
-      </c>
-      <c r="I9">
-        <v>14</v>
-      </c>
-      <c r="J9">
-        <v>18</v>
-      </c>
-      <c r="K9" s="2">
-        <f>ROUND(AVERAGE(H9:J9),0)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K12" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4">
+        <f>1/(1+SQRT(($C$4-C5)^2+($D$4-D5)^2+($E$4-E5)^2+($F$4-F5)^2+($G$4-G5)^2))</f>
+        <v>0.16076774302686761</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4">
+        <f>1/(1+SQRT(($C$4-$C6)^2+($D$4-$D6)^2+($E$4-$E6)^2+($F$4-$F6)^2+($G$4-$G6)^2))</f>
+        <v>0.19404996501286384</v>
+      </c>
+      <c r="D14" s="4">
+        <f>1/(1+SQRT(($C$5-$C6)^2+($D$5-$D6)^2+($E$5-$E6)^2+($F$5-$F6)^2+($G$5-$G6)^2)+($H$5-$H6)^2)</f>
+        <v>0.15725992956937823</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4">
+        <f>1/(1+SQRT(+($D$4-D7)^2+($F$4-F7)^2+($G$4-G7)^2))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D15" s="4">
+        <f>1/(1+SQRT(($D$5-$D7)^2+($F$5-$F7)^2+($G$5-$G7)^2)+($H$5-$H7)^2)</f>
+        <v>0.125</v>
+      </c>
+      <c r="E15" s="4">
+        <f>1/(1+SQRT(($D$6-$D7)^2+($F$6-$F7)^2+($G$6-$G7)^2)+($H$6-$H7)^2)</f>
+        <v>0.19371294336139652</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4">
+        <f>1/(1+SQRT(($C$4-C8)^2+($E$4-E8)^2+($F$4-F8)^2+($G$4-G8)^2))</f>
+        <v>0.27081318457076031</v>
+      </c>
+      <c r="D16" s="4">
+        <f>1/(1+SQRT(($C$5-$C8)^2+($E$5-$E8)^2+($F$5-$F8)^2+($G$5-$G8)^2))</f>
+        <v>0.28989794855663564</v>
+      </c>
+      <c r="E16" s="4">
+        <f>1/(1+SQRT(($C$6-$C8)^2+($E$6-$E8)^2+($F$6-$F8)^2+($G$6-$G8)^2))</f>
+        <v>0.41421356237309509</v>
+      </c>
+      <c r="F16" s="4">
+        <f>1/(1+SQRT(($F$7-$F8)^2+($G$7-$G8)^2))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4">
+        <f>C13</f>
+        <v>0.16076774302686761</v>
+      </c>
+      <c r="E21" s="4">
+        <f>C21*D21</f>
+        <v>0.32153548605373522</v>
+      </c>
+      <c r="F21" s="4">
+        <f>D16</f>
+        <v>0.28989794855663564</v>
+      </c>
+      <c r="G21" s="4">
+        <f>C21*F21</f>
+        <v>0.57979589711327129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" ref="D22:D23" si="0">C14</f>
+        <v>0.19404996501286384</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" ref="E22:E23" si="1">C22*D22</f>
+        <v>0.58214989503859149</v>
+      </c>
+      <c r="F22" s="4">
+        <f>E16</f>
+        <v>0.41421356237309509</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" ref="G22:G23" si="2">C22*F22</f>
+        <v>1.2426406871192852</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="4">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F23" s="4">
+        <f>F16</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>SUM(D21:D23)</f>
+        <v>0.68815104137306471</v>
+      </c>
+      <c r="E24">
+        <f>SUM(E21:E23)</f>
+        <v>2.2370187144256599</v>
+      </c>
+      <c r="F24">
+        <f>SUM(F21:F23)</f>
+        <v>1.0374448442630639</v>
+      </c>
+      <c r="G24">
+        <f>SUM(G21:G23)</f>
+        <v>3.1557699175658898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="6">
+        <f>E24/D24</f>
+        <v>3.2507670263233872</v>
+      </c>
+      <c r="G25" s="6">
+        <f>G24/F24</f>
+        <v>3.0418676568849805</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
empezando capitulo 3 corregida la division de palabras con tilde
</commit_message>
<xml_diff>
--- a/CAPITULO 2/Ejemplo recomendaciones.xlsx
+++ b/CAPITULO 2/Ejemplo recomendaciones.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,6 +25,65 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ivan</author>
+  </authors>
+  <commentList>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+todos los pearson negativos se computan como cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+solo se suman las similitudes de los que han votado por ese item
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
   <si>
@@ -118,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +210,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +234,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -306,6 +385,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,11 +667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,10 +802,10 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="4">
         <v>2</v>
       </c>
@@ -733,7 +815,7 @@
       <c r="F9" s="4">
         <v>4</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -899,12 +981,12 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="18">
         <f>D18/D19</f>
         <v>4.0836867836211797</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="7">
+      <c r="F20" s="18">
         <f>F18/F19</f>
         <v>3.4514162296451358</v>
       </c>
@@ -1085,12 +1167,12 @@
       <c r="A32" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="18">
         <f>D30/D31</f>
         <v>4.2220077220077226</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="F32" s="7">
+      <c r="F32" s="18">
         <f>F30/F31</f>
         <v>3.0855855855855863</v>
       </c>
@@ -1098,6 +1180,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1105,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:G16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,4 +1564,259 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>(B4-B5)^2</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D6" si="0">(C4-C5)^2</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>SUM(B6:D6)</f>
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f>1/(1+SQRT(E6))</f>
+        <v>0.41421356237309509</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>(B9-B10)^2</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11" si="1">(C9-C10)^2</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11" si="2">(D9-D10)^2</f>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>SUM(B11:D11)</f>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f>1/(1+SQRT(E11))</f>
+        <v>0.36602540378443865</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>(B14-B15)^2</f>
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16" si="3">(C14-C15)^2</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16" si="4">(D14-D15)^2</f>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f>SUM(B16:D16)</f>
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <f>1/(1+SQRT(E16))</f>
+        <v>0.1827439976315568</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>(B19-B20)^2</f>
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21" si="5">(C19-C20)^2</f>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:E21" si="6">(D19-D20)^2</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f>SUM(B21:E21)</f>
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <f>1/(1+SQRT(F21))</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>(B24-B25)^2</f>
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26" si="7">(C24-C25)^2</f>
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26" si="8">(D24-D25)^2</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26" si="9">(E24-E25)^2</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>SUM(B26:E26)</f>
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <f>1/(1+SQRT(F26))</f>
+        <v>0.26120387496374142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>